<commit_message>
Updated with first example Aircraft
</commit_message>
<xml_diff>
--- a/PythonFolder/ReferenceAircraft_inputs.xlsx
+++ b/PythonFolder/ReferenceAircraft_inputs.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mians\Desktop\TU Delft\Course 2020-2021\KBE\Assignment\Code\KBE\PythonFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{082A11D0-FD48-4540-A9FD-444058D1ED93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9851B34-7728-40F2-B2B3-1735615478F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16635" yWindow="-16170" windowWidth="18405" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>Airplane</t>
   </si>
@@ -178,6 +187,9 @@
   </si>
   <si>
     <t>LINK INFORMATION</t>
+  </si>
+  <si>
+    <t>WingLoading</t>
   </si>
 </sst>
 </file>
@@ -4204,10 +4216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M39"/>
+  <dimension ref="B1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4216,7 +4228,7 @@
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
@@ -4232,7 +4244,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -4269,8 +4281,11 @@
       <c r="M2" t="s">
         <v>49</v>
       </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -4307,8 +4322,12 @@
       <c r="M3">
         <v>2678</v>
       </c>
+      <c r="N3">
+        <f>C3/H3</f>
+        <v>659.23076923076928</v>
+      </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -4345,8 +4364,12 @@
       <c r="M4">
         <v>2702</v>
       </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N39" si="0">C4/H4</f>
+        <v>689.04109589041093</v>
+      </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -4383,8 +4406,12 @@
       <c r="M5">
         <v>2071</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>527.86885245901635</v>
+      </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -4421,8 +4448,12 @@
       <c r="M6">
         <v>2423</v>
       </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>605.73770491803282</v>
+      </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -4459,8 +4490,12 @@
       <c r="M7">
         <v>2590</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>732.78688524590166</v>
+      </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -4494,8 +4529,12 @@
       <c r="M8">
         <v>3146</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>636.08815426997251</v>
+      </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -4532,8 +4571,12 @@
       <c r="M9">
         <v>2906</v>
       </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>600.27548209366387</v>
+      </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -4570,8 +4613,12 @@
       <c r="M10">
         <v>4224</v>
       </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>710.46831955922869</v>
+      </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -4608,8 +4655,12 @@
       <c r="M11">
         <v>4242</v>
       </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>622.19679633867281</v>
+      </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -4643,8 +4694,12 @@
       <c r="M12">
         <v>4144</v>
       </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>837.29977116704811</v>
+      </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -4678,8 +4733,12 @@
       <c r="M13">
         <v>3912</v>
       </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>837.29977116704811</v>
+      </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -4713,8 +4772,12 @@
       <c r="M14">
         <v>3947</v>
       </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>534.68197879858656</v>
+      </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -4748,8 +4811,12 @@
       <c r="M15">
         <v>1788</v>
       </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>556.02150537634407</v>
+      </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -4786,8 +4853,12 @@
       <c r="M16">
         <v>3918</v>
       </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>601.44303797468353</v>
+      </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -4824,8 +4895,12 @@
       <c r="M17">
         <v>2537</v>
       </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>575.71428571428567</v>
+      </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -4862,8 +4937,12 @@
       <c r="M18">
         <v>2196</v>
       </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>620.54945054945051</v>
+      </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>19</v>
       </c>
@@ -4900,8 +4979,12 @@
       <c r="M19">
         <v>2506</v>
       </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>690.32967032967031</v>
+      </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -4938,8 +5021,12 @@
       <c r="M20">
         <v>2024</v>
       </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>575.71428571428567</v>
+      </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -4976,8 +5063,12 @@
       <c r="M21">
         <v>3859</v>
       </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>524.91935483870964</v>
+      </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -5011,8 +5102,12 @@
       <c r="L22">
         <v>89</v>
       </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>559.67741935483866</v>
+      </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -5046,8 +5141,12 @@
       <c r="L23">
         <v>107</v>
       </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>630.80645161290317</v>
+      </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -5081,8 +5180,12 @@
       <c r="L24">
         <v>209</v>
       </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>665.74363992172209</v>
+      </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -5119,8 +5222,12 @@
       <c r="M25">
         <v>4212</v>
       </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>739.41291585127203</v>
+      </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -5157,8 +5264,12 @@
       <c r="M26">
         <v>4579</v>
       </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>755.86666666666667</v>
+      </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -5195,8 +5306,12 @@
       <c r="M27">
         <v>2474</v>
       </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>626.48648648648646</v>
+      </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>28</v>
       </c>
@@ -5230,8 +5345,12 @@
       <c r="M28">
         <v>2778</v>
       </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>29</v>
       </c>
@@ -5268,8 +5387,12 @@
       <c r="M29">
         <v>2347</v>
       </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>480.84098939929328</v>
+      </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>30</v>
       </c>
@@ -5306,8 +5429,12 @@
       <c r="M30">
         <v>3249</v>
       </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>620.28268551236749</v>
+      </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>31</v>
       </c>
@@ -5344,8 +5471,12 @@
       <c r="M31">
         <v>2868</v>
       </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>552.96466431095405</v>
+      </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -5382,8 +5513,12 @@
       <c r="M32">
         <v>3123</v>
       </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>641.12014134275614</v>
+      </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -5414,8 +5549,12 @@
       <c r="L33">
         <v>400</v>
       </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>669.67523364485976</v>
+      </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -5446,8 +5585,12 @@
       <c r="L34">
         <v>400</v>
       </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>699.34579439252332</v>
+      </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>35</v>
       </c>
@@ -5481,8 +5624,12 @@
       <c r="L35">
         <v>342</v>
       </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>566.98598130841117</v>
+      </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -5516,8 +5663,12 @@
       <c r="L36">
         <v>373</v>
       </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>670.32009345794393</v>
+      </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>37</v>
       </c>
@@ -5548,8 +5699,12 @@
       <c r="L37">
         <v>413</v>
       </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>699.34579439252332</v>
+      </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>38</v>
       </c>
@@ -5580,8 +5735,12 @@
       <c r="L38">
         <v>436</v>
       </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>731.13317757009349</v>
+      </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>39</v>
       </c>
@@ -5611,6 +5770,10 @@
       </c>
       <c r="L39">
         <v>423</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>699.46261682242994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included some pictures and error fixing
</commit_message>
<xml_diff>
--- a/PythonFolder/ReferenceAircraft_inputs.xlsx
+++ b/PythonFolder/ReferenceAircraft_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mians\Desktop\TU Delft\Course 2020-2021\KBE\Assignment\Code\KBE\PythonFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9851B34-7728-40F2-B2B3-1735615478F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51665D2-2D4C-46FA-BCEE-BB2F36658CEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16635" yWindow="-16170" windowWidth="18405" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18870" yWindow="-12990" windowWidth="14730" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Airplane</t>
   </si>
@@ -191,6 +191,18 @@
   <si>
     <t>WingLoading</t>
   </si>
+  <si>
+    <t>INFORMATION TO CORRECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engines very small </t>
+  </si>
+  <si>
+    <t>Fuel tanks seem small</t>
+  </si>
+  <si>
+    <t>Engines small corrected</t>
+  </si>
 </sst>
 </file>
 
@@ -233,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -250,12 +262,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -264,6 +356,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1871,109 +1978,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>4000</c:v>
+                  <c:v>7408</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4300</c:v>
+                  <c:v>7963.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1900</c:v>
+                  <c:v>3518.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2700</c:v>
+                  <c:v>5000.4000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2700</c:v>
+                  <c:v>5000.4000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6370</c:v>
+                  <c:v>11797.24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4500</c:v>
+                  <c:v>8334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7350</c:v>
+                  <c:v>13612.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7150</c:v>
+                  <c:v>13241.800000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8500</c:v>
+                  <c:v>15742</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7500</c:v>
+                  <c:v>13890</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1375</c:v>
+                  <c:v>2546.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2400</c:v>
+                  <c:v>4444.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1900</c:v>
+                  <c:v>3518.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2850</c:v>
+                  <c:v>5278.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2700</c:v>
+                  <c:v>5000.4000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1700</c:v>
+                  <c:v>3148.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3191</c:v>
+                  <c:v>5909.732</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3197</c:v>
+                  <c:v>5920.8440000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2897</c:v>
+                  <c:v>5365.2440000000006</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5000</c:v>
+                  <c:v>9260</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6500</c:v>
+                  <c:v>12038</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7100</c:v>
+                  <c:v>13149.2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4000</c:v>
+                  <c:v>7408</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3220</c:v>
+                  <c:v>5963.4400000000005</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6805</c:v>
+                  <c:v>12602.86</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4020</c:v>
+                  <c:v>7445.04</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5760</c:v>
+                  <c:v>10667.52</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7625</c:v>
+                  <c:v>14121.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8420</c:v>
+                  <c:v>15593.84</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4820</c:v>
+                  <c:v>8926.6400000000012</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7380</c:v>
+                  <c:v>13667.76</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7455</c:v>
+                  <c:v>13806.66</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7970</c:v>
+                  <c:v>14760.44</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5604</c:v>
+                  <c:v>10378.608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3844,16 +3957,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3880,16 +3993,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3916,16 +4029,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4216,19 +4329,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N39"/>
+  <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
@@ -4244,7 +4360,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -4284,8 +4400,14 @@
       <c r="N2" t="s">
         <v>51</v>
       </c>
+      <c r="O2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -4296,7 +4418,7 @@
         <v>375</v>
       </c>
       <c r="E3">
-        <v>4000</v>
+        <v>7408</v>
       </c>
       <c r="F3">
         <v>0.82</v>
@@ -4317,7 +4439,8 @@
         <v>48</v>
       </c>
       <c r="L3">
-        <v>257</v>
+        <f>257*J3</f>
+        <v>514</v>
       </c>
       <c r="M3">
         <v>2678</v>
@@ -4326,8 +4449,16 @@
         <f>C3/H3</f>
         <v>659.23076923076928</v>
       </c>
+      <c r="O3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -4338,7 +4469,7 @@
         <v>280</v>
       </c>
       <c r="E4">
-        <v>4300</v>
+        <v>7963.6</v>
       </c>
       <c r="F4">
         <v>0.84</v>
@@ -4359,7 +4490,8 @@
         <v>48</v>
       </c>
       <c r="L4">
-        <v>231</v>
+        <f>231*2</f>
+        <v>462</v>
       </c>
       <c r="M4">
         <v>2702</v>
@@ -4368,8 +4500,16 @@
         <f t="shared" ref="N4:N39" si="0">C4/H4</f>
         <v>689.04109589041093</v>
       </c>
+      <c r="O4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -4380,7 +4520,7 @@
         <v>153</v>
       </c>
       <c r="E5">
-        <v>1900</v>
+        <v>3518.8</v>
       </c>
       <c r="F5">
         <v>0.89</v>
@@ -4401,7 +4541,8 @@
         <v>48</v>
       </c>
       <c r="L5">
-        <v>99.7</v>
+        <f>99.7*2</f>
+        <v>199.4</v>
       </c>
       <c r="M5">
         <v>2071</v>
@@ -4410,8 +4551,12 @@
         <f t="shared" si="0"/>
         <v>527.86885245901635</v>
       </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="9"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -4422,7 +4567,7 @@
         <v>179</v>
       </c>
       <c r="E6">
-        <v>2700</v>
+        <v>5000.4000000000005</v>
       </c>
       <c r="F6">
         <v>0.82</v>
@@ -4443,7 +4588,8 @@
         <v>48</v>
       </c>
       <c r="L6">
-        <v>111.2</v>
+        <f>111.2*2</f>
+        <v>222.4</v>
       </c>
       <c r="M6">
         <v>2423</v>
@@ -4452,8 +4598,12 @@
         <f t="shared" si="0"/>
         <v>605.73770491803282</v>
       </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -4464,7 +4614,7 @@
         <v>220</v>
       </c>
       <c r="E7">
-        <v>2700</v>
+        <v>5000.4000000000005</v>
       </c>
       <c r="F7">
         <v>0.82</v>
@@ -4485,7 +4635,8 @@
         <v>48</v>
       </c>
       <c r="L7">
-        <v>142</v>
+        <f>2*142</f>
+        <v>284</v>
       </c>
       <c r="M7">
         <v>2590</v>
@@ -4494,8 +4645,12 @@
         <f t="shared" si="0"/>
         <v>732.78688524590166</v>
       </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -4506,7 +4661,7 @@
         <v>380</v>
       </c>
       <c r="E8">
-        <v>6370</v>
+        <v>11797.24</v>
       </c>
       <c r="F8">
         <v>0.86</v>
@@ -4533,8 +4688,12 @@
         <f t="shared" si="0"/>
         <v>636.08815426997251</v>
       </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -4545,7 +4704,7 @@
         <v>440</v>
       </c>
       <c r="E9">
-        <v>4500</v>
+        <v>8334</v>
       </c>
       <c r="F9">
         <v>0.86</v>
@@ -4575,8 +4734,12 @@
         <f t="shared" si="0"/>
         <v>600.27548209366387</v>
       </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -4587,7 +4750,7 @@
         <v>440</v>
       </c>
       <c r="E10">
-        <v>7350</v>
+        <v>13612.2</v>
       </c>
       <c r="F10">
         <v>0.86</v>
@@ -4617,8 +4780,12 @@
         <f t="shared" si="0"/>
         <v>710.46831955922869</v>
       </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="9"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -4629,7 +4796,7 @@
         <v>440</v>
       </c>
       <c r="E11">
-        <v>7150</v>
+        <v>13241.800000000001</v>
       </c>
       <c r="F11">
         <v>0.86</v>
@@ -4659,8 +4826,12 @@
         <f t="shared" si="0"/>
         <v>622.19679633867281</v>
       </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="9"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -4671,7 +4842,7 @@
         <v>440</v>
       </c>
       <c r="E12">
-        <v>8500</v>
+        <v>15742</v>
       </c>
       <c r="F12">
         <v>0.86</v>
@@ -4698,8 +4869,12 @@
         <f t="shared" si="0"/>
         <v>837.29977116704811</v>
       </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -4710,7 +4885,7 @@
         <v>475</v>
       </c>
       <c r="E13">
-        <v>7500</v>
+        <v>13890</v>
       </c>
       <c r="F13">
         <v>0.86</v>
@@ -4737,8 +4912,12 @@
         <f t="shared" si="0"/>
         <v>837.29977116704811</v>
       </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="9"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -4747,6 +4926,9 @@
       </c>
       <c r="D14">
         <v>219</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0.9</v>
@@ -4776,8 +4958,12 @@
         <f t="shared" si="0"/>
         <v>534.68197879858656</v>
       </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -4788,7 +4974,7 @@
         <v>110</v>
       </c>
       <c r="E15">
-        <v>1375</v>
+        <v>2546.5</v>
       </c>
       <c r="F15">
         <v>0.76</v>
@@ -4815,8 +5001,12 @@
         <f t="shared" si="0"/>
         <v>556.02150537634407</v>
       </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -4827,7 +5017,7 @@
         <v>189</v>
       </c>
       <c r="E16">
-        <v>2400</v>
+        <v>4444.8</v>
       </c>
       <c r="F16">
         <v>0.9</v>
@@ -4857,8 +5047,12 @@
         <f t="shared" si="0"/>
         <v>601.44303797468353</v>
       </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -4869,7 +5063,7 @@
         <v>130</v>
       </c>
       <c r="E17">
-        <v>1900</v>
+        <v>3518.8</v>
       </c>
       <c r="F17">
         <v>0.84</v>
@@ -4899,8 +5093,12 @@
         <f t="shared" si="0"/>
         <v>575.71428571428567</v>
       </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -4911,7 +5109,7 @@
         <v>149</v>
       </c>
       <c r="E18">
-        <v>2850</v>
+        <v>5278.2</v>
       </c>
       <c r="F18">
         <v>0.82</v>
@@ -4941,8 +5139,12 @@
         <f t="shared" si="0"/>
         <v>620.54945054945051</v>
       </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>19</v>
       </c>
@@ -4953,7 +5155,7 @@
         <v>170</v>
       </c>
       <c r="E19">
-        <v>2700</v>
+        <v>5000.4000000000005</v>
       </c>
       <c r="F19">
         <v>0.82</v>
@@ -4983,8 +5185,12 @@
         <f t="shared" si="0"/>
         <v>690.32967032967031</v>
       </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -4995,7 +5201,7 @@
         <v>130</v>
       </c>
       <c r="E20">
-        <v>1700</v>
+        <v>3148.4</v>
       </c>
       <c r="F20">
         <v>0.82</v>
@@ -5025,8 +5231,12 @@
         <f t="shared" si="0"/>
         <v>575.71428571428567</v>
       </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="9"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -5037,7 +5247,7 @@
         <v>132</v>
       </c>
       <c r="E21">
-        <v>3191</v>
+        <v>5909.732</v>
       </c>
       <c r="F21">
         <v>0.84</v>
@@ -5067,8 +5277,12 @@
         <f t="shared" si="0"/>
         <v>524.91935483870964</v>
       </c>
+      <c r="O21" s="7"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="9"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -5079,7 +5293,7 @@
         <v>149</v>
       </c>
       <c r="E22">
-        <v>3197</v>
+        <v>5920.8440000000001</v>
       </c>
       <c r="F22">
         <v>0.84</v>
@@ -5106,8 +5320,12 @@
         <f t="shared" si="0"/>
         <v>559.67741935483866</v>
       </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="9"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -5118,7 +5336,7 @@
         <v>189</v>
       </c>
       <c r="E23">
-        <v>2897</v>
+        <v>5365.2440000000006</v>
       </c>
       <c r="F23">
         <v>0.84</v>
@@ -5145,8 +5363,12 @@
         <f t="shared" si="0"/>
         <v>630.80645161290317</v>
       </c>
+      <c r="O23" s="7"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="9"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -5157,7 +5379,7 @@
         <v>516</v>
       </c>
       <c r="E24">
-        <v>5000</v>
+        <v>9260</v>
       </c>
       <c r="F24">
         <v>0.92</v>
@@ -5184,8 +5406,12 @@
         <f t="shared" si="0"/>
         <v>665.74363992172209</v>
       </c>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -5196,7 +5422,7 @@
         <v>516</v>
       </c>
       <c r="E25">
-        <v>6500</v>
+        <v>12038</v>
       </c>
       <c r="F25">
         <v>0.92</v>
@@ -5226,8 +5452,12 @@
         <f t="shared" si="0"/>
         <v>739.41291585127203</v>
       </c>
+      <c r="O25" s="7"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="9"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -5238,7 +5468,7 @@
         <v>660</v>
       </c>
       <c r="E26">
-        <v>7100</v>
+        <v>13149.2</v>
       </c>
       <c r="F26">
         <v>0.92</v>
@@ -5268,8 +5498,12 @@
         <f t="shared" si="0"/>
         <v>755.86666666666667</v>
       </c>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -5280,7 +5514,7 @@
         <v>239</v>
       </c>
       <c r="E27">
-        <v>4000</v>
+        <v>7408</v>
       </c>
       <c r="F27">
         <v>0.86</v>
@@ -5310,8 +5544,12 @@
         <f t="shared" si="0"/>
         <v>626.48648648648646</v>
       </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>28</v>
       </c>
@@ -5320,6 +5558,9 @@
       </c>
       <c r="D28">
         <v>289</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0.86</v>
@@ -5349,8 +5590,12 @@
         <f t="shared" si="0"/>
         <v>662</v>
       </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="9"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>29</v>
       </c>
@@ -5361,7 +5606,7 @@
         <v>255</v>
       </c>
       <c r="E29">
-        <v>3220</v>
+        <v>5963.4400000000005</v>
       </c>
       <c r="F29">
         <v>0.86</v>
@@ -5391,8 +5636,12 @@
         <f t="shared" si="0"/>
         <v>480.84098939929328</v>
       </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="9"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>30</v>
       </c>
@@ -5403,7 +5652,7 @@
         <v>255</v>
       </c>
       <c r="E30">
-        <v>6805</v>
+        <v>12602.86</v>
       </c>
       <c r="F30">
         <v>0.86</v>
@@ -5433,8 +5682,12 @@
         <f t="shared" si="0"/>
         <v>620.28268551236749</v>
       </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>31</v>
       </c>
@@ -5445,7 +5698,7 @@
         <v>290</v>
       </c>
       <c r="E31">
-        <v>4020</v>
+        <v>7445.04</v>
       </c>
       <c r="F31">
         <v>0.86</v>
@@ -5475,8 +5728,12 @@
         <f t="shared" si="0"/>
         <v>552.96466431095405</v>
       </c>
+      <c r="O31" s="7"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="9"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -5487,7 +5744,7 @@
         <v>290</v>
       </c>
       <c r="E32">
-        <v>5760</v>
+        <v>10667.52</v>
       </c>
       <c r="F32">
         <v>0.86</v>
@@ -5517,8 +5774,12 @@
         <f t="shared" si="0"/>
         <v>641.12014134275614</v>
       </c>
+      <c r="O32" s="7"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="9"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -5529,7 +5790,7 @@
         <v>330</v>
       </c>
       <c r="E33">
-        <v>7625</v>
+        <v>14121.5</v>
       </c>
       <c r="F33">
         <v>0.87</v>
@@ -5553,8 +5814,12 @@
         <f t="shared" si="0"/>
         <v>669.67523364485976</v>
       </c>
+      <c r="O33" s="7"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="9"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -5565,7 +5830,7 @@
         <v>330</v>
       </c>
       <c r="E34">
-        <v>8420</v>
+        <v>15593.84</v>
       </c>
       <c r="F34">
         <v>0.87</v>
@@ -5589,8 +5854,12 @@
         <f t="shared" si="0"/>
         <v>699.34579439252332</v>
       </c>
+      <c r="O34" s="7"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="9"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>35</v>
       </c>
@@ -5601,7 +5870,7 @@
         <v>440</v>
       </c>
       <c r="E35">
-        <v>4820</v>
+        <v>8926.6400000000012</v>
       </c>
       <c r="F35">
         <v>0.87</v>
@@ -5628,8 +5897,12 @@
         <f t="shared" si="0"/>
         <v>566.98598130841117</v>
       </c>
+      <c r="O35" s="7"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="9"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -5640,7 +5913,7 @@
         <v>440</v>
       </c>
       <c r="E36">
-        <v>7380</v>
+        <v>13667.76</v>
       </c>
       <c r="F36">
         <v>0.87</v>
@@ -5667,8 +5940,12 @@
         <f t="shared" si="0"/>
         <v>670.32009345794393</v>
       </c>
+      <c r="O36" s="7"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="9"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>37</v>
       </c>
@@ -5679,7 +5956,7 @@
         <v>440</v>
       </c>
       <c r="E37">
-        <v>7455</v>
+        <v>13806.66</v>
       </c>
       <c r="F37">
         <v>0.87</v>
@@ -5703,8 +5980,12 @@
         <f t="shared" si="0"/>
         <v>699.34579439252332</v>
       </c>
+      <c r="O37" s="7"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="9"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>38</v>
       </c>
@@ -5715,7 +5996,7 @@
         <v>440</v>
       </c>
       <c r="E38">
-        <v>7970</v>
+        <v>14760.44</v>
       </c>
       <c r="F38">
         <v>0.87</v>
@@ -5739,8 +6020,12 @@
         <f t="shared" si="0"/>
         <v>731.13317757009349</v>
       </c>
+      <c r="O38" s="7"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="9"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>39</v>
       </c>
@@ -5751,7 +6036,7 @@
         <v>550</v>
       </c>
       <c r="E39">
-        <v>5604</v>
+        <v>10378.608</v>
       </c>
       <c r="F39">
         <v>0.87</v>
@@ -5775,10 +6060,15 @@
         <f t="shared" si="0"/>
         <v>699.46261682242994</v>
       </c>
+      <c r="O39" s="10"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:M1"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>